<commit_message>
Update ERD, 테이블 설계
</commit_message>
<xml_diff>
--- a/02.설계/StudyStory 테이블설계서_v0402.xlsx
+++ b/02.설계/StudyStory 테이블설계서_v0402.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="22575" windowHeight="6210" tabRatio="862" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="22575" windowHeight="6210" tabRatio="862" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="2.ss_user" sheetId="17" r:id="rId3"/>
     <sheet name="3.ss_question" sheetId="18" r:id="rId4"/>
     <sheet name="4.ss_alarm" sheetId="19" r:id="rId5"/>
-    <sheet name="5.ss_new_study" sheetId="20" r:id="rId6"/>
+    <sheet name="5.ss_admin_user" sheetId="20" r:id="rId6"/>
     <sheet name="6.ss_study" sheetId="21" r:id="rId7"/>
     <sheet name="7.ss_member" sheetId="22" r:id="rId8"/>
     <sheet name="8.ss_join" sheetId="23" r:id="rId9"/>
@@ -884,6 +884,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+DEFAULT 'no_user_img.png'</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G16" authorId="0">
       <text>
         <r>
@@ -1692,6 +1716,68 @@
     <author>owner</author>
   </authors>
   <commentList>
+    <comment ref="G3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+'</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>공지사항</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>', '</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>스터디</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">' </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G6" authorId="0">
       <text>
         <r>
@@ -1857,549 +1943,6 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>신촌</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>홍대</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>종각</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>건대</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>노원</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>강남</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>언어</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>취업</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>취미</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">, </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>기타</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-DEFAULT 'N'
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>관리자가</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>거절</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>시</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>거절</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>사유를</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>알림으로</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>전달</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>알림테이블에</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>추가</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>수락</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>시</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> ss_new_study </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>레코드</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">삭제
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ss_study</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>에</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>레코드</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>추가</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
 DEFAULT SYSDATE</t>
         </r>
       </text>
@@ -2635,6 +2178,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+DEFAULT 'no_study_img.png'</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G9" authorId="0">
       <text>
         <r>
@@ -3040,6 +2607,328 @@
             <family val="2"/>
           </rPr>
           <t>)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+DEFAULT 'N'
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>관리자가</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>거절</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>거절</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사유를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>알림으로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>전달</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>알림테이블에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>추가</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>수락</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> ss_new_study </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>레코드</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">삭제
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ss_study</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>레코드</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>추가</t>
         </r>
       </text>
     </comment>
@@ -3432,7 +3321,7 @@
     <author>owner</author>
   </authors>
   <commentList>
-    <comment ref="G6" authorId="0">
+    <comment ref="G7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3697,7 +3586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0">
+    <comment ref="G9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3726,7 +3615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="178">
   <si>
     <t>비고</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3896,10 +3785,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>새 스터디</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>좋아하는 스터디</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3936,10 +3821,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ss_new_study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ss_member</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4000,10 +3881,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공지사항 코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>제목</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4092,10 +3969,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>desc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>deactivation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4132,10 +4005,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>문의코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4232,14 +4101,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공지사항 코드를 만드는 시퀀스, 함수 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문의코드용 시퀀스, 함수 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>q_000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4260,14 +4121,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Entity : ss_new_study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ns_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>accept_flag</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4276,26 +4129,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>새 스터디 코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>신청일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새 스터디 코드 용 시퀀스, 함수 필요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ns_000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Entity : ss_member</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4409,6 +4246,86 @@
   </si>
   <si>
     <t>완료여부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항 번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항 번호를 만드는 시퀀스, 함수 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문의번호용 시퀀스, 함수 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알림 번호용 시퀀스, 함수 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLOB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 아이디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entity : ss_admin_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss_admin_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 유저</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4850,7 +4767,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4883,10 +4800,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -4927,10 +4844,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>42</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4949,10 +4866,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4960,10 +4877,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4971,10 +4888,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4982,10 +4899,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4993,10 +4910,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -5004,10 +4921,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -5015,10 +4932,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -5050,7 +4967,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5087,7 +5004,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -5102,7 +5019,7 @@
         <v>23</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5113,7 +5030,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>15</v>
@@ -5153,7 +5070,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5190,10 +5107,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>300</v>
@@ -5203,7 +5120,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5211,18 +5128,18 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5233,7 +5150,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3">
         <v>15</v>
@@ -5253,7 +5170,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
@@ -5268,7 +5185,7 @@
         <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -5280,10 +5197,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5297,7 +5214,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5334,7 +5251,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -5349,7 +5266,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5360,7 +5277,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
@@ -5370,7 +5287,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5378,10 +5295,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3">
         <v>100</v>
@@ -5391,7 +5308,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5399,20 +5316,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="3">
-        <v>300</v>
+        <v>167</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>168</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5420,22 +5337,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D7" s="3">
-        <v>8</v>
+        <v>300</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5443,28 +5358,51 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" t="s">
-        <v>162</v>
+      <c r="D9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="s">
-        <v>163</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -5493,7 +5431,7 @@
   <sheetData>
     <row r="1" spans="9:15">
       <c r="I1" s="4" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -5530,10 +5468,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L3" s="3">
         <v>300</v>
@@ -5543,7 +5481,7 @@
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="9:15">
@@ -5551,18 +5489,18 @@
         <v>2</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="9:15">
@@ -5573,7 +5511,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L5" s="3">
         <v>15</v>
@@ -5593,7 +5531,7 @@
         <v>4</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>15</v>
@@ -5608,7 +5546,7 @@
         <v>23</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5637,7 +5575,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5677,7 +5615,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
@@ -5697,10 +5635,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
@@ -5710,7 +5648,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5718,7 +5656,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -5729,7 +5667,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5737,10 +5675,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D6" s="3">
         <v>9</v>
@@ -5752,7 +5690,7 @@
         <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5767,7 +5705,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5782,7 +5720,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -5819,7 +5757,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -5834,7 +5772,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -5845,7 +5783,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
@@ -5855,7 +5793,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5863,20 +5801,20 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5884,18 +5822,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5903,28 +5841,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5943,7 +5881,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5955,7 +5893,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6015,7 +5953,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -6028,7 +5966,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -6036,7 +5974,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
@@ -6049,7 +5987,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6060,7 +5998,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3">
         <v>100</v>
@@ -6070,7 +6008,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6084,7 +6022,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>17</v>
@@ -6099,10 +6037,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="3">
         <v>150</v>
@@ -6112,7 +6050,7 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6120,10 +6058,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3">
         <v>150</v>
@@ -6133,7 +6071,7 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6144,7 +6082,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3">
         <v>13</v>
@@ -6175,7 +6113,7 @@
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -6183,10 +6121,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
@@ -6196,7 +6134,7 @@
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -6204,10 +6142,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="3">
         <v>100</v>
@@ -6236,7 +6174,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -6244,10 +6182,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3">
         <v>300</v>
@@ -6255,7 +6193,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -6263,7 +6201,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>15</v>
@@ -6274,7 +6212,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -6282,7 +6220,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
@@ -6291,17 +6229,17 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="B21" s="11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="B22" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -6329,7 +6267,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6343,7 +6281,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6380,7 +6318,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -6395,7 +6333,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>101</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6406,7 +6344,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
@@ -6424,10 +6362,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3">
         <v>12</v>
@@ -6437,7 +6375,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6445,20 +6383,20 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -6466,13 +6404,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -6485,7 +6423,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>15</v>
@@ -6496,7 +6434,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -6504,18 +6442,18 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -6526,7 +6464,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3">
         <v>15</v>
@@ -6543,12 +6481,12 @@
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -6560,10 +6498,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6576,7 +6514,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6613,20 +6551,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -6637,7 +6575,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>300</v>
@@ -6655,10 +6593,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3">
         <v>300</v>
@@ -6668,7 +6606,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -6676,13 +6614,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -6695,7 +6633,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -6706,7 +6644,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -6717,7 +6655,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="3">
         <v>15</v>
@@ -6730,21 +6668,55 @@
       </c>
       <c r="G8" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6756,9 +6728,9 @@
     <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -6767,7 +6739,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -6786,22 +6758,20 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3">
         <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>17</v>
@@ -6810,21 +6780,21 @@
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>17</v>
@@ -6833,165 +6803,28 @@
         <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="3">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="3">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="3">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="3">
-        <v>15</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>141</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -7005,8 +6838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -7019,7 +6852,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7056,7 +6889,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>15</v>
@@ -7071,7 +6904,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -7079,10 +6912,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>72</v>
@@ -7094,7 +6927,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7102,10 +6935,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D5" s="3">
         <v>6</v>
@@ -7115,7 +6948,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7123,10 +6956,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D6" s="3">
         <v>6</v>
@@ -7136,7 +6969,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7144,20 +6977,20 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7168,17 +7001,15 @@
         <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -7186,7 +7017,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>15</v>
@@ -7197,7 +7028,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -7205,18 +7036,18 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -7224,7 +7055,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>15</v>
@@ -7235,7 +7066,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -7246,7 +7077,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="3">
         <v>15</v>
@@ -7258,17 +7089,36 @@
         <v>23</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -7296,7 +7146,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7336,7 +7186,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
@@ -7345,7 +7195,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>
@@ -7356,7 +7206,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
@@ -7368,10 +7218,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -7399,7 +7249,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7439,7 +7289,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3">
         <v>15</v>
@@ -7448,7 +7298,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>
@@ -7459,7 +7309,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>15</v>
@@ -7471,10 +7321,10 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -7482,10 +7332,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3">
         <v>300</v>
@@ -7495,7 +7345,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -7503,10 +7353,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3">
         <v>300</v>
@@ -7516,7 +7366,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -7524,7 +7374,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -7535,7 +7385,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7543,20 +7393,20 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>